<commit_message>
Added new Class Diagram and ViewHistory diagram Probably going to be one of the last commits :(
</commit_message>
<xml_diff>
--- a/_FinalPlanning/BurnDown/Burn Down Weekly.xlsx
+++ b/_FinalPlanning/BurnDown/Burn Down Weekly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Git\BehrmanCSE248\_FinalPlanning\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8753F0CC-2D3A-4859-A100-3581FD25770C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D531785-9BF0-4D80-B210-64BD91480DDE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9465" xr2:uid="{DA367FED-CA60-4BF4-8911-7275EB64BDF3}"/>
   </bookViews>
@@ -228,48 +228,9 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -282,12 +243,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF12B2B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1736,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7ED47F-6869-4BC4-B1B1-05FD05CC8E29}">
   <dimension ref="C4:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S35" sqref="S35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,862 +1755,763 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>43402</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>43410</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>43416</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>43423</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>43430</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>43437</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>43444</v>
       </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
     </row>
     <row r="5" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="20">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
         <v>1</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="7">
         <v>2</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="7">
         <v>3</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="7">
         <v>4</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="7">
         <v>5</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="7">
         <v>6</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="7">
         <v>7</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="2"/>
     </row>
     <row r="6" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="18">
         <v>20</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="12">
         <v>12</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="9">
         <v>3</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="12">
         <v>3</v>
       </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8">
-        <v>0</v>
-      </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
-      <c r="N6" s="8">
-        <v>0</v>
-      </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
+      <c r="K6" s="12">
+        <v>0</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
     </row>
     <row r="8" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="18">
         <v>3</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="9">
         <v>3</v>
       </c>
-      <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="13">
-        <v>0</v>
-      </c>
-      <c r="K8" s="13">
-        <v>0</v>
-      </c>
-      <c r="L8" s="13">
-        <v>0</v>
-      </c>
-      <c r="M8" s="13">
-        <v>0</v>
-      </c>
-      <c r="N8" s="13">
-        <v>0</v>
-      </c>
-      <c r="O8" s="17"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+      <c r="N8" s="9">
+        <v>0</v>
+      </c>
+      <c r="O8" s="4"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
     </row>
     <row r="9" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="18">
         <v>3</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="8">
-        <v>0</v>
-      </c>
-      <c r="M10" s="8">
-        <v>0</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="17"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
+      <c r="J10" s="12">
+        <v>0</v>
+      </c>
+      <c r="K10" s="12">
+        <v>0</v>
+      </c>
+      <c r="L10" s="12">
+        <v>0</v>
+      </c>
+      <c r="M10" s="12">
+        <v>0</v>
+      </c>
+      <c r="N10" s="12">
+        <v>0</v>
+      </c>
+      <c r="O10" s="4"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
     </row>
     <row r="11" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="7">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="18">
         <v>5</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="12">
         <v>5</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <v>0</v>
-      </c>
-      <c r="M12" s="8">
-        <v>0</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="17"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
+      <c r="J12" s="12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="12">
+        <v>0</v>
+      </c>
+      <c r="L12" s="12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
     </row>
     <row r="13" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="7">
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="18">
         <v>10</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="12">
         <v>10</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="9">
         <v>8</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="12">
         <v>2</v>
       </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>0</v>
-      </c>
-      <c r="M14" s="8">
-        <v>0</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="18">
         <v>5</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="9">
         <v>5</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="9">
         <v>5</v>
       </c>
-      <c r="J16" s="13">
-        <v>0</v>
-      </c>
-      <c r="K16" s="13">
-        <v>0</v>
-      </c>
-      <c r="L16" s="13">
-        <v>0</v>
-      </c>
-      <c r="M16" s="13">
-        <v>0</v>
-      </c>
-      <c r="N16" s="13">
-        <v>0</v>
-      </c>
-      <c r="O16" s="17"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="9">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
     </row>
     <row r="17" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
     </row>
     <row r="18" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="7">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="18">
         <v>7</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="9">
         <v>7</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="9">
         <v>7</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="9">
         <v>7</v>
       </c>
-      <c r="K18" s="13">
-        <v>0</v>
-      </c>
-      <c r="L18" s="13">
-        <v>0</v>
-      </c>
-      <c r="M18" s="13">
-        <v>0</v>
-      </c>
-      <c r="N18" s="13">
-        <v>0</v>
-      </c>
-      <c r="O18" s="17"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0</v>
+      </c>
+      <c r="N18" s="9">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
     </row>
     <row r="19" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="17"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
     </row>
     <row r="20" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="18">
         <v>7</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="9">
         <v>7</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="9">
         <v>7</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="9">
         <v>7</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="9">
         <v>7</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="9">
         <v>1</v>
       </c>
-      <c r="M20" s="13">
-        <v>0</v>
-      </c>
-      <c r="N20" s="13">
-        <v>0</v>
-      </c>
-      <c r="O20" s="17"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
+      <c r="M20" s="9">
+        <v>0</v>
+      </c>
+      <c r="N20" s="9">
+        <v>0</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
     </row>
     <row r="21" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="17"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
     </row>
     <row r="22" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="7">
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="18">
         <v>5</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="9">
         <v>5</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="9">
         <v>5</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="9">
         <v>5</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="9">
         <v>3</v>
       </c>
-      <c r="L22" s="13">
+      <c r="L22" s="9">
         <v>3</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="9">
         <v>2</v>
       </c>
-      <c r="N22" s="13">
-        <v>0</v>
-      </c>
-      <c r="O22" s="17"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
-      <c r="S22" s="16"/>
+      <c r="N22" s="9">
+        <v>0</v>
+      </c>
+      <c r="O22" s="4"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
     </row>
     <row r="23" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7">
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="18">
         <v>10</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="12">
         <v>10</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="9">
         <v>10</v>
       </c>
-      <c r="J24" s="8">
-        <v>0</v>
-      </c>
-      <c r="K24" s="8">
-        <v>0</v>
-      </c>
-      <c r="L24" s="8">
-        <v>0</v>
-      </c>
-      <c r="M24" s="8">
-        <v>0</v>
-      </c>
-      <c r="N24" s="8">
-        <v>0</v>
-      </c>
-      <c r="O24" s="17"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0</v>
+      </c>
+      <c r="N24" s="12">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
     </row>
     <row r="26" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="13">
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="9">
         <f>SUM(G6:G25)</f>
         <v>75</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="9">
         <f t="shared" ref="H26" si="0">SUM(H6:H25)</f>
         <v>67</v>
       </c>
-      <c r="I26" s="13">
-        <f>SUM(I6:I25)</f>
+      <c r="I26" s="9">
+        <f t="shared" ref="I26:N26" si="1">SUM(I6:I25)</f>
         <v>47</v>
       </c>
-      <c r="J26" s="13">
-        <f>SUM(J6:J25)</f>
+      <c r="J26" s="9">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="K26" s="13">
-        <f>SUM(K6:K25)</f>
+      <c r="K26" s="9">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L26" s="13">
-        <f>SUM(L6:L25)</f>
+      <c r="L26" s="9">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M26" s="13">
-        <f>SUM(M6:M25)</f>
+      <c r="M26" s="9">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="N26" s="13">
-        <f>SUM(N6:N25)</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="17"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
+      <c r="N26" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="4"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
     </row>
     <row r="27" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="13">
-        <f>SUM(G6:G24)</f>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9">
+        <f>SUM(G5:G24)</f>
         <v>75</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="9">
         <f>MAX(G28-11,0)</f>
         <v>64</v>
       </c>
-      <c r="I28" s="13">
-        <f t="shared" ref="I28:N28" si="1">MAX(H28-11,0)</f>
+      <c r="I28" s="9">
+        <f>MAX(H28-11,0)</f>
         <v>53</v>
       </c>
-      <c r="J28" s="13">
-        <f t="shared" si="1"/>
+      <c r="J28" s="9">
+        <f t="shared" ref="J28:N28" si="2">MAX(I28-11,0)</f>
         <v>42</v>
       </c>
-      <c r="K28" s="13">
-        <f t="shared" si="1"/>
+      <c r="K28" s="9">
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="L28" s="13">
-        <f t="shared" si="1"/>
+      <c r="L28" s="9">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="M28" s="13">
-        <f t="shared" si="1"/>
+      <c r="M28" s="9">
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N28" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="18"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
+      <c r="N28" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="5"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
-      <c r="S29" s="19"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="109">
-    <mergeCell ref="C28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="C26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="C24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="C22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="C20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="C18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="C16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="C14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="C12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="C10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="C8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
@@ -2616,9 +2522,111 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="C8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="C10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="C12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="C14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="C16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="C18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="C20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="C22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="C24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="C26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="C28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G26:N26" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>